<commit_message>
improved buttons size, made some basic balancing of units and enemies
</commit_message>
<xml_diff>
--- a/MyAssets/Balance.xlsx
+++ b/MyAssets/Balance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="22995" windowHeight="9285"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="22992" windowHeight="9288"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Fishing Boat</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>Friendly</t>
+  </si>
+  <si>
+    <t>Enemy</t>
+  </si>
+  <si>
+    <t>Damage to ship</t>
   </si>
 </sst>
 </file>
@@ -383,18 +392,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D4:J9"/>
+  <dimension ref="D3:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:10">
+    <row r="3" spans="4:11">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="4:11">
       <c r="E4" t="s">
         <v>4</v>
       </c>
@@ -414,7 +428,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="4:10">
+    <row r="5" spans="4:11">
       <c r="D5" t="s">
         <v>0</v>
       </c>
@@ -424,8 +438,8 @@
       <c r="F5">
         <v>0.3</v>
       </c>
-      <c r="G5" t="s">
-        <v>9</v>
+      <c r="G5">
+        <v>25</v>
       </c>
       <c r="H5" t="s">
         <v>9</v>
@@ -434,10 +448,10 @@
         <v>9</v>
       </c>
       <c r="J5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="4:10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11">
       <c r="D6" t="s">
         <v>1</v>
       </c>
@@ -448,7 +462,7 @@
         <v>0.3</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <v>0.8</v>
@@ -457,10 +471,10 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="4:10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11">
       <c r="D7" t="s">
         <v>2</v>
       </c>
@@ -468,65 +482,131 @@
         <v>20</v>
       </c>
       <c r="F7">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G7">
         <v>2</v>
       </c>
       <c r="H7">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="I7">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="J7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="4:10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11">
       <c r="D8" t="s">
         <v>10</v>
       </c>
       <c r="E8">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F8">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H8">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="4:10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11">
       <c r="D9" t="s">
         <v>3</v>
       </c>
       <c r="E9">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F9">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>0.95</v>
+      </c>
+      <c r="I9">
+        <v>1.5</v>
+      </c>
+      <c r="J9">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11">
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11">
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11">
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>0.3</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>0.8</v>
+      </c>
+      <c r="I15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11">
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" t="s">
         <v>10</v>
       </c>
-      <c r="H9">
-        <v>0.7</v>
-      </c>
-      <c r="I9">
-        <v>4</v>
-      </c>
-      <c r="J9">
-        <v>40</v>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -540,7 +620,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -552,7 +632,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>